<commit_message>
Before class report config changes
</commit_message>
<xml_diff>
--- a/com.demowebshop_maven/src/test/resources/TestData/TestData.xlsx
+++ b/com.demowebshop_maven/src/test/resources/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>yogbelavanaki@gmail.com</t>
   </si>
@@ -71,13 +71,10 @@
     <t>Victoria</t>
   </si>
   <si>
-    <t>david002@manchesterunited.com</t>
-  </si>
-  <si>
-    <t>victoriabeckham002@spicegirls.com</t>
-  </si>
-  <si>
-    <t>Passwor@123</t>
+    <t>david003@manchesterunited.com</t>
+  </si>
+  <si>
+    <t>victoriabeckham003@spicegirls.com</t>
   </si>
 </sst>
 </file>
@@ -430,7 +427,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,7 +557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -583,7 +580,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>